<commit_message>
Added variables to variable_key.xlsx
</commit_message>
<xml_diff>
--- a/data/variable_key.xlsx
+++ b/data/variable_key.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="319">
   <si>
     <t>VCF0004</t>
   </si>
@@ -341,6 +341,1190 @@
 --------------
 00. NA; DK; RF; no Pre IW
 INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0102</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Age Group</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  17 - 24
+2.  25 - 34
+3.  35 - 44
+4.  45 - 54
+5.  55 - 64
+6.  65 - 74
+7.  75 - 99 and over (except 1954)
+MISSING_CODES:
+--------------
+0.  NA; DK; RF; no Pre IW
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0104</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Gender</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Male
+2.  Female
+MISSING_CODES:
+--------------
+0.  NA; no Pre IW</t>
+  </si>
+  <si>
+    <t>VCF0105a</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1. White non-Hispanic (1948-2012)
+2. Black non-Hispanic (1948-2012)
+3. Asian or Pacific Islander, non-Hispanic (1966-2012)
+4. American Indian or Alaska Native non-Hispanic (1966-2012)
+5. Hispanic (1966-2012)
+6. Other or multiple races, non-Hispanic (1968-2012)
+7. Non-white and non-black (1948-1964)
+MISSING_CODES:
+--------------
+9. Missing</t>
+  </si>
+  <si>
+    <t>Race-ethnicity summary, 7 categories</t>
+  </si>
+  <si>
+    <t>VCF0105b</t>
+  </si>
+  <si>
+    <t>Race-ethnicity summary, 4 categories</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1. White non-Hispanic
+2. Black non-Hispanic
+3. Hispanic
+4. Other or multiple races, non-Hispanic
+MISSING_CODES:
+--------------
+9. Missing, DK/REF/NA
+0. Missing, pre-1966 data
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0110</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Education 4-category</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Grade school or less (0-8 grades)
+2.  High school (12 grades or fewer, incl. non-college
+      training if applicable)
+3.  Some college (13 grades or more but no degree; 
+      1948 ONLY: college, no identification of degree
+      status)
+4.  College or advanced degree (no cases 1948)
+MISSING_CODES:
+--------------
+0.  DK; NA; no Pre IW; short-form 'new' Cross Section 
+    (1992)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0111</t>
+  </si>
+  <si>
+    <t>SAMPLE DESCRIPTION: Urbanism</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Central cities
+2.  Suburban areas
+3.  Rural, small towns, outlying and adjacent areas
+MISSING_CODES:
+--------------
+0.  NA; telephone (RDD) sample (2000)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0112</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Northeast (CT, ME, MA, NH, NJ, NY, PA, RI, VT)
+2.  North Central (IL, IN, IA, KS, MI, MN, MO, NE, ND,
+      OH, SD, WI)
+3.  South (AL, AR, DE, D.C., FL, GA, KY, LA, MD, MS, NC
+      OK, SC,TN, TX, VA, WV)
+4.  West (AK, AZ, CA, CO, HI, ID, MT, NV, NM, OR, UT, WA, 
+      WY)
+MISSING_CODES:
+--------------
+0.  NA (1948)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>SAMPLE DESCRIPTION: Census Region</t>
+  </si>
+  <si>
+    <t>VCF0113</t>
+  </si>
+  <si>
+    <t>SAMPLE DESCRIPTION: Political South/Nonsouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALID_CODES:
+------------
+1.  South
+2.  Nonsouth
+</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  0 to 16 percentile
+2.  17 to 33 percentile
+3.  34 to 67 percentile
+4.  68 to 95 percentile
+5.  96 to 100 percentile
+MISSING_CODES:
+--------------
+0.  DK; NA; refused to answer; no Pre IW
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0114</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent Family - Income Group</t>
+  </si>
+  <si>
+    <t>VCF0115</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Occupation Group 6-category</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Professional and managerial
+2.  Clerical and sales workers
+3.  Skilled, semi-skilled and service workers
+4.  Laborers, except farm
+5.  Farmers, farm managers, farm laborers and foremen;
+      forestry and fishermen
+6.  Homemakers (1972-1992: 7 IN VCF0116, 4 in VCF0118;
+      1952-1970: 4 in VCF0118)
+MISSING_CODES:
+--------------
+0.  NA; member of armed forces; no occupation and not a 
+    homemaker; no Pre IW
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0116</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Work Status 7-category</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Working now
+2.  Temporarily laid off
+4.  Unemployed
+5.  Retired 
+6.  Permanently disabled 
+7.  Homemaker 
+8.  Student
+MISSING_CODES:
+--------------
+9. NA; DK
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0117</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Head of HH - Work Status 7-category 1948-1986</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Working now
+2.  Temporarily laid off
+4.  Unemployed (1972 adds "looking for work.")
+5.  Retired
+6.  Permanently disabled 
+7.  Housewife (not working at least 20 hrs. per wk.)
+8.  Student (not working at least 20 hrs. per wk.)
+MISSING_CODES:
+--------------
+9.  NA; DK
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0126</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Father of Respondent - Occupation 5-category 1952-1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+VALID_CODES:
+------------
+1.  Professional and managerial
+2.  Clerical and sales workers
+3.  Skilled, semi-skilled and service workers
+4.  Laborers, except farm
+5.  Farmers, farm managers, farm laborers and foremen
+MISSING_CODES:
+--------------
+0.  DK; NA; father wasn't living/not raised by father/no
+    information for parental surrogate; member of armed
+    forces; father not in labor force; no Pre IW;
+    short-form or Spanish language (1992)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Religion Major Group</t>
+  </si>
+  <si>
+    <t>VCF0128</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Protestant
+2.  Catholic [Roman Catholic]
+3.  Jewish
+4.  Other and none (also includes DK preference)
+MISSING_CODES:
+--------------
+0.  DK; NA; refused to answer; no Pre IW; no Post IW; 
+    short-form 'new' Cross Section (1992)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0131</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Church Attendance 1952-1968</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Regularly
+2.  Often
+4.  Seldom
+5.  Never
+7.  No religious preference (1960-1968)
+MISSING_CODES:
+--------------
+9.  NA
+0.  Religion refused/NA; no Pre IW; no Post IW
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0138</t>
+  </si>
+  <si>
+    <t>HOUSEHOLD COMPOSITION: Number of Children</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+0.  None
+1.  One
+2.  Two
+3.  Three or more
+MISSING_CODES:
+--------------
+9.  NA; no Pre IW; Panel (1992,1996,2002)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0140a</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Education 7-category</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  8 grades or less ('grade school')
+2.  9-12 grades ('high school'), no diploma/equivalency
+3.  12 grades, diploma or equivalency
+4.  12 grades, diploma or equivalency plus non-academic
+      training
+5.  Some college, no degree; junior/community college
+      level degree (AA degree)
+6.  BA level degrees
+7.  Advanced degrees incl. LLB
+MISSING_CODES:
+--------------
+8.  DK
+9.  NA; RF; no Pre IW; short-form 'new' Cross Section (1992)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0146</t>
+  </si>
+  <si>
+    <t>(Do you/ Does your family) own your own home, pay rent or what?</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Yes, own
+2.  No, not owned
+MISSING_CODES:
+--------------
+8.  DK
+9.  NA; RF; no Pre IW; short form (1992)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Marital Status</t>
+  </si>
+  <si>
+    <t>VCF0147</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Married
+2.  Never married
+3.  Divorced
+4.  Separated
+5.  Widowed
+7.  Partners; not married (VOLUNTEERED [exc.1986,2012])
+MISSING_CODES:
+--------------
+8.  R not married/partnered, refused to say whether never
+      married, divorced, separated or widowed (1992
+      only); DK
+9.  NA; no Pre IW; unmarried at time of IW (1952 only);
+      short-form 'new' Cross-Section (1992)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>There's been some talk these days about different social classes.
+Most people say they belong either to the middle class or the working
+class.
+Do you ever think of yourself as belonging in one of these classes?</t>
+  </si>
+  <si>
+    <t>VCF0148</t>
+  </si>
+  <si>
+    <t>(IF YES:) Which one? / 
+(IF NO:) Well, if you had to make a  choice, would you call yourself
+middle class or working class?  Would you say that you are about
+average middle/working class or that you are in the upper part of the
+middle/working class?
+VALID_CODES:
+------------
+0.  Lower class (VOLUNTEERED)
+1.  Average working
+2.  Working--NA average or upper
+3.  Upper working
+4.  Average middle
+5.  Middle class--NA average or upper
+6.  Upper middle
+7.  Upper class (VOLUNTEERED)
+MISSING_CODES:
+--------------
+9.  DK; NA; other (incl. "refused to accept idea of
+    class")
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0154b</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Occupation 14-category</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Executive, administrative and managerial
+2.  Professional specialty occupations
+3.  Technicians and related support occupations
+4.  Sales occupation
+5.  Administrative support, including clerical
+6.  Private household
+7.  Protective service
+8.  Service except protective and household
+9.  Farming, forestry and fishing occupations
+10. Precision production, craft and repair occupations
+11. Machine operators, assemblers and inspectors
+12. Transportation and material moving occupations
+13. Handlers, equipment cleaners, helpers and laborers
+14. Member of armed forces
+MISSING_CODES:
+--------------
+00.   DK; NA; honworking homemaker/student; R has never 
+worked for pay
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0155</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Worried about Find/Losing Job</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  A lot
+3.  Somewhat
+5.  Not much at all
+MISSING_CODES:
+--------------
+8.  DK; refused
+9.  NA
+0.  R is nonworking homemaker or student; R is 
+    unemployed/disabled and has never worked for pay, or
+    R is working and retired (1984-1986); R is
+    unemployed/disabled and has never worked for pay, or
+    R is working and retired/disabled (1988-1994); R is
+    unemployed/disabled and has never worked for pay
+    (1996-1998)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0156</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Yes
+5.  No
+MISSING_CODES:
+--------------
+8.  DK
+9.  NA
+0.  R is not currently working
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>DEMOGRAPHICS: Respondent - Working R Laid off Last 6 Months</t>
+  </si>
+  <si>
+    <t>VCF0157</t>
+  </si>
+  <si>
+    <t>During the last six months, have you had a reduction in your
+work hours or had to take a cut in pay at any time for reasons
+other than illness or personal choice?</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Democrats</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+00-96. Degrees as coded
+97. 97-100 Degrees
+MISSING_CODES:
+--------------
+98. DK  (exc. 1964-1968: see VCF0201 note)
+99. NA; no Post IW; form III,IV (1972)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0201</t>
+  </si>
+  <si>
+    <t>VCF0202</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Republicans</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Protestants</t>
+  </si>
+  <si>
+    <t>VCF0203</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Catholics</t>
+  </si>
+  <si>
+    <t>VCF0204</t>
+  </si>
+  <si>
+    <t>VCF0205</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Jews</t>
+  </si>
+  <si>
+    <t>VCF0206</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Blacks</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Whites</t>
+  </si>
+  <si>
+    <t>VCF0207</t>
+  </si>
+  <si>
+    <t>VCF0208</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Southerners</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Big Business</t>
+  </si>
+  <si>
+    <t>VCF0209</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Labor Unions</t>
+  </si>
+  <si>
+    <t>VCF0210</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Liberals</t>
+  </si>
+  <si>
+    <t>VCF0211</t>
+  </si>
+  <si>
+    <t>VCF0212</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Conservatives</t>
+  </si>
+  <si>
+    <t>VCF0213</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Military</t>
+  </si>
+  <si>
+    <t>VCF0214</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Policemen</t>
+  </si>
+  <si>
+    <t>VCF0215</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Black Militants</t>
+  </si>
+  <si>
+    <t>VCF0216</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Civil Rights Leaders</t>
+  </si>
+  <si>
+    <t>VCF0217</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Chicanos/Hispanics</t>
+  </si>
+  <si>
+    <t>VCF0218</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Democratic Party</t>
+  </si>
+  <si>
+    <t>VCF0219</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Middle Class People</t>
+  </si>
+  <si>
+    <t>VCF0220</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: People on Welfare</t>
+  </si>
+  <si>
+    <t>VCF0221</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Political Independents</t>
+  </si>
+  <si>
+    <t>VCF0222</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Political Parties</t>
+  </si>
+  <si>
+    <t>VCF0223</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Poor People</t>
+  </si>
+  <si>
+    <t>VCF0224</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Republican Party</t>
+  </si>
+  <si>
+    <t>VCF0225</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Womens Libbers</t>
+  </si>
+  <si>
+    <t>VCF0226</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Young People</t>
+  </si>
+  <si>
+    <t>VCF0227</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Asian-Americans</t>
+  </si>
+  <si>
+    <t>VCF0228</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Congress</t>
+  </si>
+  <si>
+    <t>VCF0229</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Environmentalists</t>
+  </si>
+  <si>
+    <t>VCF0230</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Anti-Abortionists</t>
+  </si>
+  <si>
+    <t>VCF0231</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Federal Government</t>
+  </si>
+  <si>
+    <t>VCF0232</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Gays and Lesbians</t>
+  </si>
+  <si>
+    <t>VCF0233</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Illegal Aliens</t>
+  </si>
+  <si>
+    <t>VCF0234</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Christian Fundamentalists</t>
+  </si>
+  <si>
+    <t>VCF0235</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Radical Students</t>
+  </si>
+  <si>
+    <t>VCF0236</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Farmers</t>
+  </si>
+  <si>
+    <t>GROUP THERMOMETER: Feminists</t>
+  </si>
+  <si>
+    <t>VCF0253</t>
+  </si>
+  <si>
+    <t>VCF0290</t>
+  </si>
+  <si>
+    <t>PARTIES: Major Party Thermometer Avg</t>
+  </si>
+  <si>
+    <t>VCF0291</t>
+  </si>
+  <si>
+    <t>PARTIES: Major Party Thermometer Index</t>
+  </si>
+  <si>
+    <t>VCF0301</t>
+  </si>
+  <si>
+    <t>PARTISANSHIP: Party Identification of Respondent- 7-point Scale</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Strong Democrat
+2.  Weak Democrat
+3.  Independent - Democrat        
+4.  Independent - Independent
+5.  Independent - Republican
+6.  Weak Republican
+7.  Strong Republican
+MISSING_CODES:
+--------------
+0.  NA/RF initial party identification; Democrat or 
+    Republican initial party identification but DK/NA/RF 
+    strength; initial party identification independent/
+    no preference/other/DK and followup is DK/NA/RF/other;
+    no Pre IW
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0303</t>
+  </si>
+  <si>
+    <t>PARTISANSHIP: Party Identification of Respondent- Summary 3-Category</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Democrats (including leaners)
+2.  Independents
+3.  Republicans (including leaners)
+MISSING_CODES:
+--------------
+0.  DK; NA; other; refused to answer; no Pre IW
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0305</t>
+  </si>
+  <si>
+    <t>PARTISANSHIP: Party Identification of Respondent- Strength of Partisanship</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Independent
+2.  Leaning Independent
+3.  Weak Partisan
+4.  Strong Partisan
+MISSING_CODES:
+--------------
+0.  DK; NA; other; refused to answer; no Pre IW
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0306</t>
+  </si>
+  <si>
+    <t>PARTISANSHIP: Party Identification of Respondent's Father</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Democrat
+2.  Independent (some years also: shifted around)
+3.  Republican
+4.  Other; minor party; apolitical; never voted, didn't
+    get into politics; parents refused to say; DK (1988  
+    only); father not a U.S. citizen
+MISSING_CODES:
+--------------
+9.  DK (exc. 1988)
+0.  NA; no Pre IW; no Post IW; R had no
+    father/father substitute; DK/NA father's interest
+    in politics (1972 only)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0310</t>
+  </si>
+  <si>
+    <t>POLITICAL INTEREST: Interest in the Elections</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Not much interested
+2.  Somewhat interested
+3.  Very much interested
+9.  DK
+MISSING_CODES:
+--------------
+0.  NA; no Pre IW; split versions: not asked (2008)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0311</t>
+  </si>
+  <si>
+    <t>POLITICAL INTEREST: Does Respondent Care Which Party Wins Presidential Election</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Don't care very much or DK, pro-con, depends, and
+    other
+2.  Care a good deal
+MISSING_CODES:
+--------------
+0.  NA; no Pre IW
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>PARTIES: Democratic Party: What Respondent Likes - Number of Mentions</t>
+  </si>
+  <si>
+    <t>VCF0314</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+0.  Zero positive mentions (likes)
+1.  One positive mention (likes)
+2.  Two positive mentions (likes)
+3.  Three positive mentions (likes)
+4.  Four positive mentions (likes)
+5.  Five positive mentions (likes)
+MISSING_CODES:
+--------------
+9.  No Pre IW; form II (1972); form B (1986); form A
+    (1990); questions not administered in assigned half
+    sample [See VCF012A] (1996)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0315</t>
+  </si>
+  <si>
+    <t>PARTIES: Democratic Party: What Respondent Dislikes - Number of Mentions</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+0.  Zero negative mentions (dislikes)
+1.  One negative mention (dislikes)
+2.  Two negative mentions (dislikes)
+3.  Three negative mentions (dislikes)
+4.  Four negative mentions (dislikes)
+5.  Five negative mentions (dislikes)
+MISSING_CODES:
+--------------
+9.  No Pre IW; form II (1972); form B (1986); form A
+    (1990); questions not administered in assigned half
+    sample [See VCF012a] (1996)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>PARTIES: Republican Party: What Respondent Likes - Number of Mentions</t>
+  </si>
+  <si>
+    <t>VCF0318</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+0.  Zero positive mentions (likes)
+1.  One positive mention (likes)
+2.  Two positive mentions (likes)
+3.  Three positive mentions (likes)
+4.  Four positive mentions (likes)
+5.  Five positive mentions (likes)
+MISSING_CODES:
+--------------
+9.  No Pre IW; form II (1972); form B (1986); form A
+    (1990); questions not administered in assigned half
+    sample [See VCF012a] (1996)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0319</t>
+  </si>
+  <si>
+    <t>PARTIES: Republican Party: What Respondent Dislikes - Number of Mentions</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+0.  Zero negative mentions (dislikes)
+1.  One negative mention (dislikes)
+2.  Two negative mentions (dislikes)
+3.  Three negative mentions (dislikes)
+4.  Four negative mentions (dislikes)
+5.  Five negative mentions (dislikes)
+MISSING_CODES:
+--------------
+9.  No Pre IW; form II (1972); form B (1986); form A
+    (1990); questions not administered in assigned half
+    sample [See VCF012A] (1996)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>VCF0320</t>
+  </si>
+  <si>
+    <t>PARTIES: Republican Party: Affect (Likes-Dislikes)</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: President- Intelligent</t>
+  </si>
+  <si>
+    <t>VCF0338</t>
+  </si>
+  <si>
+    <t>VALID_CODES:
+------------
+1.  Extremely well
+2.  Quite well
+3.  Not too well
+4.  Not well at all
+MISSING_CODES:
+--------------
+8.  DK
+9.  NA
+0.  Form B (1986); R selected for Post 
+    administration and no Post IW (2000); R not selected 
+    for this trait (2002); no Post IW; split versions: 
+    not asked (2008)
+INAP. Inap. question not used</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: President- Compassionate</t>
+  </si>
+  <si>
+    <t>VCF0339</t>
+  </si>
+  <si>
+    <t>VCF0340</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: President- Decent</t>
+  </si>
+  <si>
+    <t>VCF0341</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: President- Inspiring</t>
+  </si>
+  <si>
+    <t>VCF0342</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: President- Knowledgeable</t>
+  </si>
+  <si>
+    <t>VCF0343</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: President- Moral</t>
+  </si>
+  <si>
+    <t>VCF0344</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: President- Leadership</t>
+  </si>
+  <si>
+    <t>VCF0345</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: President- Cares</t>
+  </si>
+  <si>
+    <t>VCF0346</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: President- Angry</t>
+  </si>
+  <si>
+    <t>VCF0347</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: President- Afraid</t>
+  </si>
+  <si>
+    <t>VCF0348</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: President- Hopeful</t>
+  </si>
+  <si>
+    <t>VCF0349</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: President- Proud</t>
+  </si>
+  <si>
+    <t>VCF0350</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Democratic Presidential Cand- Intelligent</t>
+  </si>
+  <si>
+    <t>VCF0351</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Democratic Presidential Cand- Compassionate</t>
+  </si>
+  <si>
+    <t>VCF0352</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Democratic Presidential Cand- Decent</t>
+  </si>
+  <si>
+    <t>VCF0353</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Democratic Presidential Cand- Inspiring</t>
+  </si>
+  <si>
+    <t>VCF0354</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Democratic Presidential Cand- Knowledgeable</t>
+  </si>
+  <si>
+    <t>VCF0355</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Democratic Presidential Cand- Moral</t>
+  </si>
+  <si>
+    <t>VCF0356</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Democratic Presidential Cand- Leadership</t>
+  </si>
+  <si>
+    <t>VCF0357</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Democratic Presidential Cand- Cares</t>
+  </si>
+  <si>
+    <t>VCF0358</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: Democratic Presidential Cand- Angry</t>
+  </si>
+  <si>
+    <t>VCF0359</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: Democratic Presidential Cand- Afraid</t>
+  </si>
+  <si>
+    <t>VCF0360</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: Democratic Presidential Cand- Hopeful</t>
+  </si>
+  <si>
+    <t>VCF0361</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: Democratic Presidential Cand- Proud</t>
+  </si>
+  <si>
+    <t>VCF0362</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Republican Presidential Cand- Intelligent</t>
+  </si>
+  <si>
+    <t>VCF0363</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Republican Presidential Cand- Compassionate</t>
+  </si>
+  <si>
+    <t>VCF0364</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Republican Presidential Cand- Decent</t>
+  </si>
+  <si>
+    <t>VCF0365</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Republican Presidential Cand- Inspiring</t>
+  </si>
+  <si>
+    <t>VCF0366</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Republican Presidential Cand- Knowledgeable</t>
+  </si>
+  <si>
+    <t>VCF0367</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Republican Presidential Cand- Moral</t>
+  </si>
+  <si>
+    <t>VCF0368</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Republican Presidential Cand- Leadership</t>
+  </si>
+  <si>
+    <t>VCF0369</t>
+  </si>
+  <si>
+    <t>CANDIDATE TRAITS: Republican Presidential Cand- Cares</t>
+  </si>
+  <si>
+    <t>VCF0370</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: Republican Presidential Cand- Angry</t>
+  </si>
+  <si>
+    <t>VCF0371</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: Republican Presidential Cand- Afraid</t>
+  </si>
+  <si>
+    <t>VCF0372</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: Republican Presidential Cand- Hopeful</t>
+  </si>
+  <si>
+    <t>VCF0373</t>
+  </si>
+  <si>
+    <t>CANDIDATE AFFECTS: Republican Presidential Cand- Proud</t>
+  </si>
+  <si>
+    <t>VCF0374</t>
+  </si>
+  <si>
+    <t>PARTIES: Likes Anything about Democratic party</t>
   </si>
 </sst>
 </file>
@@ -699,10 +1883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,6 +2134,1002 @@
         <v>61</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="270" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>153</v>
+      </c>
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>160</v>
+      </c>
+      <c r="B61" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>162</v>
+      </c>
+      <c r="B62" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>164</v>
+      </c>
+      <c r="B63" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>166</v>
+      </c>
+      <c r="B64" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>168</v>
+      </c>
+      <c r="B65" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>174</v>
+      </c>
+      <c r="B68" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>176</v>
+      </c>
+      <c r="B69" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>180</v>
+      </c>
+      <c r="B71" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>182</v>
+      </c>
+      <c r="B72" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>184</v>
+      </c>
+      <c r="B73" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>188</v>
+      </c>
+      <c r="B75" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>190</v>
+      </c>
+      <c r="B76" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>192</v>
+      </c>
+      <c r="B77" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>194</v>
+      </c>
+      <c r="B78" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>196</v>
+      </c>
+      <c r="B79" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>200</v>
+      </c>
+      <c r="B81" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>202</v>
+      </c>
+      <c r="B82" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>204</v>
+      </c>
+      <c r="B83" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>207</v>
+      </c>
+      <c r="B84" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>208</v>
+      </c>
+      <c r="B85" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>210</v>
+      </c>
+      <c r="B86" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="270" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>212</v>
+      </c>
+      <c r="B87" t="s">
+        <v>213</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>215</v>
+      </c>
+      <c r="B88" t="s">
+        <v>216</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>218</v>
+      </c>
+      <c r="B89" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>221</v>
+      </c>
+      <c r="B90" t="s">
+        <v>222</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>224</v>
+      </c>
+      <c r="B91" t="s">
+        <v>225</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>227</v>
+      </c>
+      <c r="B92" t="s">
+        <v>228</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>231</v>
+      </c>
+      <c r="B93" t="s">
+        <v>230</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>233</v>
+      </c>
+      <c r="B94" t="s">
+        <v>234</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>237</v>
+      </c>
+      <c r="B95" t="s">
+        <v>236</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>239</v>
+      </c>
+      <c r="B96" t="s">
+        <v>240</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>242</v>
+      </c>
+      <c r="B97" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>245</v>
+      </c>
+      <c r="B98" t="s">
+        <v>244</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>248</v>
+      </c>
+      <c r="B99" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>249</v>
+      </c>
+      <c r="B100" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>251</v>
+      </c>
+      <c r="B101" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>253</v>
+      </c>
+      <c r="B102" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>255</v>
+      </c>
+      <c r="B103" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>257</v>
+      </c>
+      <c r="B104" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>259</v>
+      </c>
+      <c r="B105" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>261</v>
+      </c>
+      <c r="B106" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>263</v>
+      </c>
+      <c r="B107" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>265</v>
+      </c>
+      <c r="B108" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>267</v>
+      </c>
+      <c r="B109" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>269</v>
+      </c>
+      <c r="B110" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>271</v>
+      </c>
+      <c r="B111" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>273</v>
+      </c>
+      <c r="B112" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>275</v>
+      </c>
+      <c r="B113" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>277</v>
+      </c>
+      <c r="B114" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>279</v>
+      </c>
+      <c r="B115" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>281</v>
+      </c>
+      <c r="B116" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>283</v>
+      </c>
+      <c r="B117" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>285</v>
+      </c>
+      <c r="B118" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>287</v>
+      </c>
+      <c r="B119" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>289</v>
+      </c>
+      <c r="B120" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>291</v>
+      </c>
+      <c r="B121" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>293</v>
+      </c>
+      <c r="B122" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>295</v>
+      </c>
+      <c r="B123" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>297</v>
+      </c>
+      <c r="B124" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>299</v>
+      </c>
+      <c r="B125" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>301</v>
+      </c>
+      <c r="B126" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>303</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>305</v>
+      </c>
+      <c r="B128" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>307</v>
+      </c>
+      <c r="B129" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>309</v>
+      </c>
+      <c r="B130" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>311</v>
+      </c>
+      <c r="B131" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>313</v>
+      </c>
+      <c r="B132" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>315</v>
+      </c>
+      <c r="B133" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>317</v>
+      </c>
+      <c r="B134" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>